<commit_message>
Adding Empty key validation
</commit_message>
<xml_diff>
--- a/src/Common_Exceptions.xlsx
+++ b/src/Common_Exceptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AmmarMansuri/IdeaProjects/safencrypt/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6DD486A-9EAD-7C47-816E-EAF735A2EE42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140181B4-3963-874D-9F0E-123E1F5F3579}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{20B01DC0-201D-0644-AEE7-704977969841}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="57">
   <si>
     <t>NoSuchAlgorithmException</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>Either the Key/IV/Associated Data used for encryption was different than provided for decryption</t>
+  </si>
+  <si>
+    <t>SAF-015</t>
+  </si>
+  <si>
+    <t>Compile Time: Unsecure Key! Key is initialized with all zeros</t>
   </si>
 </sst>
 </file>
@@ -556,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{237002A0-E58F-A14D-986E-0E61662BC1FA}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -726,16 +732,19 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -746,7 +755,7 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
         <v>41</v>
@@ -763,7 +772,7 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
         <v>41</v>
@@ -780,7 +789,7 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
         <v>41</v>
@@ -791,19 +800,19 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -814,7 +823,7 @@
         <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
         <v>52</v>
@@ -831,7 +840,7 @@
         <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D18" t="s">
         <v>52</v>
@@ -842,19 +851,24 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>